<commit_message>
update ce decile table for ISA model
</commit_message>
<xml_diff>
--- a/data/Conditional Survival Prob Feb 16.xlsx
+++ b/data/Conditional Survival Prob Feb 16.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Quintus/Google Drive/Dynamic Programming/code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidhya Balakrishnan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21F41CE-8794-43D2-AE6E-D125B58041C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,21 +28,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>AGE</t>
   </si>
   <si>
     <t>CSP</t>
   </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -82,6 +80,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -349,16 +350,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -366,651 +367,667 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>22</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>0.99932270553865132</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>0.99930200799150271</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>24</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>0.99931165031836178</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>25</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>0.99933143569120431</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>26</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>0.99936139803148405</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>27</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>0.99938127599147986</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>28</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>0.9993859644671339</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>29</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>0.99938051254969862</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>0.99934963976139912</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>31</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>0.99931871450578835</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>32</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>0.9992877275456109</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>33</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>0.99924648955777085</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>34</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <v>0.99918987496560785</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>35</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>0.9991229233169816</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>36</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>0.99905580450559883</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>37</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>0.99897317483103365</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>38</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>0.99889541186818576</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>39</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>0.99880715909323614</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>40</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>0.99871346707808384</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>41</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>0.99861429737178398</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>42</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>0.99851472681766085</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>43</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>0.99840956934843816</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>44</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>0.99831424182123751</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>45</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>0.99821327136586624</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>46</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>0.99810143607995694</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>47</v>
       </c>
-      <c r="B29">
+      <c r="B31">
         <v>0.99798380827001421</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>48</v>
       </c>
-      <c r="B30">
+      <c r="B32">
         <v>0.9978758543324262</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>49</v>
       </c>
-      <c r="B31">
+      <c r="B33">
         <v>0.99777244598962211</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>50</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>0.99767358158895425</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>51</v>
       </c>
-      <c r="B33">
+      <c r="B35">
         <v>0.99756358978380777</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>52</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>0.99742138364779875</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>53</v>
       </c>
-      <c r="B35">
+      <c r="B37">
         <v>0.99724656872017992</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>54</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>0.99702294701899519</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>55</v>
       </c>
-      <c r="B37">
+      <c r="B39">
         <v>0.99676038473734274</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>56</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>0.99645824386157456</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>57</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>0.9961157609649941</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>58</v>
       </c>
-      <c r="B40">
+      <c r="B42">
         <v>0.99575875091475308</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>59</v>
       </c>
-      <c r="B41">
+      <c r="B43">
         <v>0.99538124818951368</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>60</v>
       </c>
-      <c r="B42">
+      <c r="B44">
         <v>0.99499334421971086</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>61</v>
       </c>
-      <c r="B43">
+      <c r="B45">
         <v>0.99455650402981199</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>62</v>
       </c>
-      <c r="B44">
+      <c r="B46">
         <v>0.99405287063359804</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>63</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>0.99345298751958622</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>64</v>
       </c>
-      <c r="B46">
+      <c r="B48">
         <v>0.99272600934203192</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>65</v>
       </c>
-      <c r="B47">
+      <c r="B49">
         <v>0.99188942959358262</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>66</v>
       </c>
-      <c r="B48">
+      <c r="B50">
         <v>0.99096061651507694</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>67</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>0.98997954085611906</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>68</v>
       </c>
-      <c r="B50">
+      <c r="B52">
         <v>0.98897610824080151</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>69</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>0.98797580151702324</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>70</v>
       </c>
-      <c r="B52">
+      <c r="B54">
         <v>0.98694719867251712</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>71</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>0.98577999846078246</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>72</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>0.98449388943938987</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>73</v>
       </c>
-      <c r="B55">
+      <c r="B57">
         <v>0.98318205109435619</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>74</v>
       </c>
-      <c r="B56">
+      <c r="B58">
         <v>0.98186443306964477</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>75</v>
       </c>
-      <c r="B57">
+      <c r="B59">
         <v>0.98046786138563813</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>76</v>
       </c>
-      <c r="B58">
+      <c r="B60">
         <v>0.97873807682392366</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>77</v>
       </c>
-      <c r="B59">
+      <c r="B61">
         <v>0.97672228733982169</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>78</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>0.97467065787522067</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>79</v>
       </c>
-      <c r="B61">
+      <c r="B63">
         <v>0.9726497381873016</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>80</v>
       </c>
-      <c r="B62">
+      <c r="B64">
         <v>0.97045123208761519</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>81</v>
       </c>
-      <c r="B63">
+      <c r="B65">
         <v>0.96797596365235239</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>82</v>
       </c>
-      <c r="B64">
+      <c r="B66">
         <v>0.96481160429710267</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>83</v>
       </c>
-      <c r="B65">
+      <c r="B67">
         <v>0.9605467585254468</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>84</v>
       </c>
-      <c r="B66">
+      <c r="B68">
         <v>0.95491491916708182</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>85</v>
       </c>
-      <c r="B67">
+      <c r="B69">
         <v>0.94814916205418642</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>86</v>
       </c>
-      <c r="B68">
+      <c r="B70">
         <v>0.94064891006207607</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>87</v>
       </c>
-      <c r="B69">
+      <c r="B71">
         <v>0.93274118978648302</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>88</v>
       </c>
-      <c r="B70">
+      <c r="B72">
         <v>0.92460048127352379</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>89</v>
       </c>
-      <c r="B71">
+      <c r="B73">
         <v>0.91625977377125756</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>90</v>
       </c>
-      <c r="B72">
+      <c r="B74">
         <v>0.90763422716954567</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>91</v>
       </c>
-      <c r="B73">
+      <c r="B75">
         <v>0.89856894476394278</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>92</v>
       </c>
-      <c r="B74">
+      <c r="B76">
         <v>0.88892031077903133</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>93</v>
       </c>
-      <c r="B75">
+      <c r="B77">
         <v>0.87852251226495659</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>94</v>
       </c>
-      <c r="B76">
+      <c r="B78">
         <v>0.86727147975909125</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>95</v>
       </c>
-      <c r="B77">
+      <c r="B79">
         <v>0.85500175808720114</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>96</v>
       </c>
-      <c r="B78">
+      <c r="B80">
         <v>0.84285200226186197</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>97</v>
       </c>
-      <c r="B79">
+      <c r="B81">
         <v>0.8309953647231032</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>98</v>
       </c>
-      <c r="B80">
+      <c r="B82">
         <v>0.81970642201834865</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>99</v>
       </c>
-      <c r="B81">
+      <c r="B83">
         <v>0.80920404691556991</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>100</v>
       </c>
-      <c r="B82">
+      <c r="B84">
         <v>0.79972337482710931</v>
       </c>
     </row>

</xml_diff>